<commit_message>
c2 due date change
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6848DB2-FF9F-B44E-B5D1-3003F11AC386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF86FC1E-5714-FD44-ADE0-9296AD44E01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>Component 1 draft</t>
   </si>
   <si>
-    <t>Component 2 draft</t>
-  </si>
-  <si>
     <t>Component 3 draft</t>
   </si>
   <si>
@@ -188,13 +185,16 @@
     <t>[Data and variables](https://soc333-sum23.github.io/slides/02-datavariables.html#/title-slide)</t>
   </si>
   <si>
-    <t>Component 1: proposal AND HW1: Getting oriented to R</t>
-  </si>
-  <si>
     <t>[Intro to the computing workflow](https://soc333-sum23.github.io/slides/03-computing.html#/title-slide)</t>
   </si>
   <si>
     <t>[Project and research questions](https://soc333-sum23.github.io/slides/04-researchquestions.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>HW 1: Getting oriented to R</t>
+  </si>
+  <si>
+    <t>Component 1: proposal</t>
   </si>
 </sst>
 </file>
@@ -563,13 +563,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AA364B-4369-6A4C-8B80-A99A4414C3D0}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="3" max="3" width="97.1640625" customWidth="1"/>
+    <col min="4" max="4" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,7 +612,7 @@
         <v>45063</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -622,13 +623,13 @@
         <v>45064</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -639,10 +640,10 @@
         <v>45068</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -650,7 +651,7 @@
         <v>45069</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -700,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -721,8 +722,8 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
-        <v>39</v>
+      <c r="F11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -739,7 +740,7 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -813,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -835,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -854,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -868,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -879,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to project proposal instructions
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B90A32C-559B-C44F-BA8D-96EB0509B3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D037ABB-739F-D445-8C60-7F780FA4D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changing due date for c2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45B94F-90EE-DD46-9E32-9B25C9B4F497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18400E-34C9-484B-ACA5-F1B94AE6ACAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16440" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Research questions</t>
   </si>
   <si>
-    <t>Making nice plots</t>
-  </si>
-  <si>
     <t>Hypothesis testing pt 1</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>[Project and research questions](https://soc333-sum23.github.io/slides/04-researchquestions.html#/title-slide)</t>
   </si>
   <si>
-    <t>HW 1: Getting oriented to R</t>
-  </si>
-  <si>
     <t>Component 1: proposal</t>
   </si>
   <si>
@@ -194,16 +188,22 @@
     <t>[Workshopping project proposals](https://soc333-sum23.github.io/slides/06-workshopping.html#/title-slide)</t>
   </si>
   <si>
-    <t>Describing data pt 2</t>
-  </si>
-  <si>
-    <t>Describing data pt 3</t>
-  </si>
-  <si>
     <t>Summary statistics</t>
   </si>
   <si>
-    <t>[Describing data pt 1](https://soc333-sum23.github.io/slides/07-describingpt1.html#/title-slide)</t>
+    <t>Summary statistics; filtering</t>
+  </si>
+  <si>
+    <t>[Describing data pt 1: Summary statistics](https://soc333-sum23.github.io/slides/07-describingpt1.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>[Describing data pt 2: Filtering data frames](https://soc333-sum23.github.io/slides/08-describingpt2.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>Describing data pt 4: Plots</t>
+  </si>
+  <si>
+    <t>Describing data pt 3: Creating new variables; plots</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AA364B-4369-6A4C-8B80-A99A4414C3D0}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,25 +585,25 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -621,10 +621,10 @@
         <v>45063</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -632,13 +632,13 @@
         <v>45064</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -649,10 +649,10 @@
         <v>45068</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>45069</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -671,10 +671,10 @@
         <v>45070</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -685,10 +685,10 @@
         <v>45071</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>45075</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -707,13 +707,13 @@
         <v>45076</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -721,10 +721,13 @@
         <v>45077</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -732,13 +735,10 @@
         <v>45078</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -749,13 +749,10 @@
         <v>45082</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -763,10 +760,13 @@
         <v>45083</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -774,7 +774,7 @@
         <v>45084</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>45085</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -793,13 +793,13 @@
         <v>45089</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>45090</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -815,10 +815,10 @@
         <v>45091</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -826,10 +826,10 @@
         <v>45092</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -840,7 +840,7 @@
         <v>45096</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -848,10 +848,10 @@
         <v>45097</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
         <v>45098</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -867,13 +867,13 @@
         <v>45099</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add slides 9 links
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18400E-34C9-484B-ACA5-F1B94AE6ACAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1298386B-33E1-294D-A3F4-53AABE353145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16440" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
@@ -203,7 +203,7 @@
     <t>Describing data pt 4: Plots</t>
   </si>
   <si>
-    <t>Describing data pt 3: Creating new variables; plots</t>
+    <t>[Describing data pt 3: Creating new variables](https://soc333-sum23.github.io/slides/09-describingpt3.html#/title-slide)</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add link to slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/Teaching essentials/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978A4DAF-65E0-044A-A11E-BB11AE4824F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1ECD6-85F6-A447-847E-935C5039C130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42140" yWindow="2240" windowWidth="28800" windowHeight="16440" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,9 +45,6 @@
     <t>Research questions</t>
   </si>
   <si>
-    <t>Hypothesis testing pt 2</t>
-  </si>
-  <si>
     <t>Best fit lines pt 1</t>
   </si>
   <si>
@@ -201,13 +193,16 @@
   </si>
   <si>
     <t>[Hypothesis testing pt 1](https://soc333-sum23.github.io/slides/13-hypothesistests1.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>[Hypothesis testing pt 2](https://soc333-sum23.github.io/slides/14-hypothesistests2.html#/title-slide)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -570,37 +565,37 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="97.1640625" customWidth="1"/>
     <col min="4" max="4" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -610,7 +605,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
@@ -618,27 +613,27 @@
         <v>45063</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="B3" s="2">
         <v>45064</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>2</v>
       </c>
@@ -646,49 +641,49 @@
         <v>45068</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="B5" s="2">
         <v>45069</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" s="2">
         <v>45070</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="B7" s="2">
         <v>45071</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>3</v>
       </c>
@@ -696,52 +691,52 @@
         <v>45075</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="2">
         <v>45076</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10" s="2">
         <v>45077</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="B11" s="2">
         <v>45078</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>4</v>
       </c>
@@ -749,43 +744,43 @@
         <v>45082</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="B13" s="2">
         <v>45083</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="B14" s="2">
         <v>45084</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="2">
         <v>45085</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>5</v>
       </c>
@@ -793,40 +788,40 @@
         <v>45089</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="B17" s="2">
         <v>45090</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="B18" s="2">
         <v>45091</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="B19" s="2">
         <v>45092</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>6</v>
       </c>
@@ -834,43 +829,43 @@
         <v>45096</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="B21" s="2">
         <v>45097</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="B22" s="2">
         <v>45098</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="B23" s="2">
         <v>45099</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>7</v>
       </c>
@@ -881,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="B25" s="2">
         <v>45105</v>
       </c>
@@ -892,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project c3 info, slides 14
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/Teaching essentials/Teaching/Soc333_sum23/soc333_github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1ECD6-85F6-A447-847E-935C5039C130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A44EBD9-F666-CD43-96A0-8F55EDFC9763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16600" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,20 +189,20 @@
     <t>[Plotting relationships between variables](https://soc333-sum23.github.io/slides/12-plots2.html#/title-slide)</t>
   </si>
   <si>
-    <t>[IMS ch 11](https://openintro-ims.netlify.app/foundations-randomization.html) and [ch 13] (https://openintro-ims.netlify.app/foundations-mathematical.html#foundations-mathematical)</t>
-  </si>
-  <si>
     <t>[Hypothesis testing pt 1](https://soc333-sum23.github.io/slides/13-hypothesistests1.html#/title-slide)</t>
   </si>
   <si>
     <t>[Hypothesis testing pt 2](https://soc333-sum23.github.io/slides/14-hypothesistests2.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>[IMS ch 11](https://openintro-ims.netlify.app/foundations-randomization.html) and [ch 13](https://openintro-ims.netlify.app/foundations-mathematical.html#foundations-mathematical)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -565,17 +565,17 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="97.1640625" customWidth="1"/>
     <col min="4" max="4" width="66.5" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -605,7 +605,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -619,7 +619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>45064</v>
       </c>
@@ -633,7 +633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -647,7 +647,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>45069</v>
       </c>
@@ -658,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>45070</v>
       </c>
@@ -672,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>45071</v>
       </c>
@@ -683,7 +683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>45076</v>
       </c>
@@ -708,7 +708,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>45077</v>
       </c>
@@ -722,7 +722,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>45078</v>
       </c>
@@ -736,7 +736,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -747,7 +747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>45083</v>
       </c>
@@ -755,7 +755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>45084</v>
       </c>
@@ -766,21 +766,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>45085</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -788,10 +788,10 @@
         <v>45089</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>45090</v>
       </c>
@@ -799,7 +799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>45091</v>
       </c>
@@ -810,7 +810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>45092</v>
       </c>
@@ -821,7 +821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -832,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>45097</v>
       </c>
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>45098</v>
       </c>
@@ -851,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>45099</v>
       </c>
@@ -865,7 +865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7</v>
       </c>
@@ -879,7 +879,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>45105</v>
       </c>

</xml_diff>

<commit_message>
slides 15, exercise solutions
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A44EBD9-F666-CD43-96A0-8F55EDFC9763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413524D-A399-3746-8549-B2F8228CED84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16600" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Best fit lines pt 2</t>
   </si>
   <si>
-    <t>Hypothesis testing pt 3</t>
-  </si>
-  <si>
     <t>Causality</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>[IMS ch 11](https://openintro-ims.netlify.app/foundations-randomization.html) and [ch 13](https://openintro-ims.netlify.app/foundations-mathematical.html#foundations-mathematical)</t>
+  </si>
+  <si>
+    <t>[Hypothesis testing pt 3](https://soc333-sum23.github.io/slides/15-hypothesistests3.html#/title-slide)</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,25 +577,25 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -613,10 +613,10 @@
         <v>45063</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -624,13 +624,13 @@
         <v>45064</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -641,10 +641,10 @@
         <v>45068</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -652,7 +652,7 @@
         <v>45069</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -663,10 +663,10 @@
         <v>45070</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -677,10 +677,10 @@
         <v>45071</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -691,7 +691,7 @@
         <v>45075</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -699,13 +699,13 @@
         <v>45076</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -713,13 +713,13 @@
         <v>45077</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -727,13 +727,13 @@
         <v>45078</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -744,7 +744,7 @@
         <v>45082</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>45083</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -760,10 +760,10 @@
         <v>45084</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -771,13 +771,13 @@
         <v>45085</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -788,7 +788,7 @@
         <v>45089</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>45090</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -829,7 +829,7 @@
         <v>45096</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -837,10 +837,10 @@
         <v>45097</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -848,7 +848,7 @@
         <v>45098</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -856,13 +856,13 @@
         <v>45099</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated instructions for paper and pres
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aidan/Desktop/School/Grad_school/Teaching/Soc333_sum23/soc333_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A9B4A-1008-474F-BD10-80F15896A18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF10847-3340-1D42-9C4A-47BDF911B695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41320" yWindow="4020" windowWidth="28800" windowHeight="16600" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
+    <workbookView xWindow="-40300" yWindow="500" windowWidth="29400" windowHeight="17280" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Final project presentations</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Getting to know you survey</t>
   </si>
   <si>
-    <t>Wrapup</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -211,6 +208,12 @@
   </si>
   <si>
     <t>[Interpreting results](https://soc333-sum23.github.io/slides/17-interpretingresults.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>Interpreting results</t>
+  </si>
+  <si>
+    <t>Final project presentations; workshop final papers</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,13 +595,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -610,7 +613,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -628,7 +631,7 @@
         <v>45063</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -639,13 +642,13 @@
         <v>45064</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -656,10 +659,10 @@
         <v>45068</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -667,7 +670,7 @@
         <v>45069</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -678,10 +681,10 @@
         <v>45070</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -692,10 +695,10 @@
         <v>45071</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -714,13 +717,13 @@
         <v>45076</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -728,13 +731,13 @@
         <v>45077</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -742,13 +745,13 @@
         <v>45078</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -759,7 +762,7 @@
         <v>45082</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -767,10 +770,10 @@
         <v>45083</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -778,10 +781,10 @@
         <v>45084</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -789,16 +792,16 @@
         <v>45085</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -809,10 +812,10 @@
         <v>45089</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -820,10 +823,10 @@
         <v>45090</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -831,10 +834,10 @@
         <v>45091</v>
       </c>
       <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
         <v>55</v>
-      </c>
-      <c r="G18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -842,10 +845,13 @@
         <v>45092</v>
       </c>
       <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -864,13 +870,13 @@
         <v>45097</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -886,13 +892,10 @@
         <v>45099</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -903,10 +906,13 @@
         <v>45103</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -917,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slides / site update
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssche\Documents\work docs\teaching\soc333-sum24.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEB2A29-9D9E-4D89-B20C-3A289DB8F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAF63B4-267F-4BAE-85A6-A752606FDDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="195" windowWidth="21600" windowHeight="11295" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
+    <workbookView xWindow="3540" yWindow="2655" windowWidth="21600" windowHeight="11295" xr2:uid="{159CD874-63CF-3B4E-8DA1-4D7FF80F5CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Final project presentations</t>
   </si>
@@ -93,9 +93,6 @@
     <t>No class (Memorial Day)</t>
   </si>
   <si>
-    <t>Pipes</t>
-  </si>
-  <si>
     <t>Plotting relationships between variables</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>[Creating new variables](https://soc333-sum24.github.io/slides/09-describingpt3.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>[Pipes](https://soc333-sum24.github.io/slides/10-describingpt4.html#/title-slide)</t>
+  </si>
+  <si>
+    <t>[Plotting one variable](https://soc333-sum24.github.io/slides/11-plots.html#/title-slide)</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AA364B-4369-6A4C-8B80-A99A4414C3D0}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -639,12 +642,12 @@
         <v>45427</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
@@ -653,7 +656,7 @@
         <v>45428</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -661,7 +664,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -670,7 +673,7 @@
         <v>45429</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="63" x14ac:dyDescent="0.25">
@@ -681,12 +684,12 @@
         <v>45432</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
@@ -695,12 +698,12 @@
         <v>45433</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
@@ -709,7 +712,7 @@
         <v>45434</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -726,10 +729,10 @@
         <v>45435</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -740,7 +743,7 @@
         <v>45436</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="1"/>
@@ -763,11 +766,11 @@
         <v>45440</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>14</v>
@@ -779,7 +782,7 @@
         <v>45441</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -787,7 +790,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
@@ -796,7 +799,7 @@
         <v>45442</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -804,7 +807,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -813,13 +816,13 @@
         <v>45443</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -827,19 +830,19 @@
         <v>45446</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="4">
         <v>45447</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -853,7 +856,7 @@
         <v>45448</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -868,17 +871,17 @@
         <v>45449</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +890,7 @@
         <v>45450</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
@@ -901,12 +904,12 @@
         <v>45453</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,12 +918,12 @@
         <v>45454</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,12 +932,12 @@
         <v>45455</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -946,7 +949,7 @@
         <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="3" t="s">
@@ -959,7 +962,7 @@
         <v>45457</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
@@ -973,11 +976,11 @@
         <v>45460</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -987,13 +990,13 @@
         <v>45461</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1004,7 +1007,7 @@
         <v>45462</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1019,7 +1022,7 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1029,7 +1032,7 @@
         <v>45464</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1043,11 +1046,11 @@
         <v>45467</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="1"/>
     </row>

</xml_diff>